<commit_message>
add the final log
</commit_message>
<xml_diff>
--- a/notebooks/convnet/logs/final_recap_reforged.xlsx
+++ b/notebooks/convnet/logs/final_recap_reforged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnau\Desktop\quatrième_année\Deep_Learning\Projet_cifar-10\saves\REAL_RESULTS\all_logs\convnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B12DAA-718E-4C00-8620-7D85461A2BA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CED6E6-B6A8-4622-A2E4-46B95607A8DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12525" yWindow="1560" windowWidth="13545" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="final_recap" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2193" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2238" uniqueCount="611">
   <si>
     <t>Test1 : Nombre de couches (bloc de 2 convs + pool)</t>
   </si>
@@ -1835,6 +1835,24 @@
   </si>
   <si>
     <t>Forte</t>
+  </si>
+  <si>
+    <t>Dernier Test</t>
+  </si>
+  <si>
+    <t>0.336</t>
+  </si>
+  <si>
+    <t>0.898</t>
+  </si>
+  <si>
+    <t>0.896</t>
+  </si>
+  <si>
+    <t>31824.99</t>
+  </si>
+  <si>
+    <t>Data aug</t>
   </si>
 </sst>
 </file>
@@ -2158,7 +2176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2273,6 +2291,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2318,9 +2367,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2680,6 +2732,41 @@
     <tableColumn id="23" xr3:uid="{881E5941-2B56-4B24-8E58-1A50CE72F656}" name="momentum"/>
     <tableColumn id="24" xr3:uid="{83FA9A07-A726-4B28-8255-9F53E3CF6F9D}" name="optimizer"/>
     <tableColumn id="25" xr3:uid="{F4775B22-C365-4AC6-B103-DD09973DA8C4}" name="batch_size"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{FBF91AA9-258F-43DE-9428-D7C6634B869A}" name="Tableau119" displayName="Tableau119" ref="A164:Z165" totalsRowShown="0">
+  <autoFilter ref="A164:Z165" xr:uid="{989EFA7C-0205-498E-8109-02601457CC46}"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{5C55095E-44EE-46E1-8C62-8E0F0E5F4A70}" name="indiv_id"/>
+    <tableColumn id="27" xr3:uid="{7A60E805-AF5C-4347-AD6F-635FD297D10C}" name="Data aug"/>
+    <tableColumn id="2" xr3:uid="{93BFDB1B-5485-4CD7-B760-20EED42E4F6A}" name="epochs"/>
+    <tableColumn id="3" xr3:uid="{91CD0627-DBE4-43E2-847E-9802FC1D01FB}" name="nb_layers"/>
+    <tableColumn id="4" xr3:uid="{A4D7C832-03BF-48B4-8AC8-FDE15146A5CD}" name="l1"/>
+    <tableColumn id="5" xr3:uid="{722F5D2C-72DB-4E0B-A226-8AA88921424E}" name="l2"/>
+    <tableColumn id="6" xr3:uid="{7C2EFC29-2DB6-430C-B78D-D3B6CCABB181}" name="batch_norm"/>
+    <tableColumn id="7" xr3:uid="{75E5FC33-02B7-4290-B27B-3325B27D3375}" name="dropout"/>
+    <tableColumn id="8" xr3:uid="{6C33C55B-4129-40E1-883D-CFF7A11CCB20}" name="filters_per_layers"/>
+    <tableColumn id="9" xr3:uid="{706F38AF-5E82-41C7-9FE0-C1C2939CA835}" name="filters_double"/>
+    <tableColumn id="10" xr3:uid="{6D72E5C6-1C56-4F87-AC01-6B32B7A057E9}" name="MLP_end"/>
+    <tableColumn id="11" xr3:uid="{8EC98DD9-5B29-4300-BED0-0ED6F0243FA7}" name="activation"/>
+    <tableColumn id="12" xr3:uid="{5CA80D7B-511A-439A-A73E-06E203E1F6AC}" name="kernel"/>
+    <tableColumn id="13" xr3:uid="{47D9E341-386E-4AE9-825B-A22E7EA5E42B}" name="padding"/>
+    <tableColumn id="14" xr3:uid="{6818E144-A77A-4055-B1B5-096AFA30C944}" name="max_or_avg_pool"/>
+    <tableColumn id="15" xr3:uid="{D14F4E09-7330-4624-9BDE-EF850A1F0CD0}" name="pool_frequency"/>
+    <tableColumn id="16" xr3:uid="{8375179C-25E5-48D4-BB4F-33584ADF33CC}" name="pool_frequency_change"/>
+    <tableColumn id="17" xr3:uid="{29BF0F2D-0896-48F4-A695-C434C46811B7}" name="loss"/>
+    <tableColumn id="18" xr3:uid="{03589FE1-F40D-492D-8CEA-285B4A634222}" name="val_loss"/>
+    <tableColumn id="19" xr3:uid="{38027795-B4AE-4047-98C9-FB42EE70F8DF}" name="accuracy"/>
+    <tableColumn id="20" xr3:uid="{1E4C30FD-E5FF-432D-96D1-6214ECFB8B21}" name="val_accuracy"/>
+    <tableColumn id="21" xr3:uid="{60657D6E-9B17-44EE-B944-84A1E40264EF}" name="time_taken"/>
+    <tableColumn id="22" xr3:uid="{F34F6347-BD8F-4E44-9841-A7E5142D0965}" name="learning_r"/>
+    <tableColumn id="23" xr3:uid="{2F24CB93-8FD3-4AAC-A7FA-B29C9C45D654}" name="momentum"/>
+    <tableColumn id="24" xr3:uid="{BC137F98-C7EE-47A8-82B7-C887E62AF06F}" name="optimizer"/>
+    <tableColumn id="25" xr3:uid="{2A7C394F-26AF-4848-9019-068853099CD5}" name="batch_size"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3255,10 +3342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z161"/>
+  <dimension ref="A1:Z165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="C164" sqref="C164"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13165,10 +13252,199 @@
         <v>189</v>
       </c>
     </row>
+    <row r="163" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="B163" s="3"/>
+      <c r="C163" s="3"/>
+      <c r="D163" s="3"/>
+      <c r="E163" s="3"/>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3"/>
+      <c r="H163" s="3"/>
+      <c r="I163" s="3"/>
+      <c r="J163" s="3"/>
+      <c r="K163" s="3"/>
+      <c r="L163" s="3"/>
+      <c r="M163" s="3"/>
+      <c r="N163" s="3"/>
+      <c r="O163" s="3"/>
+      <c r="P163" s="3"/>
+      <c r="Q163" s="3"/>
+      <c r="R163" s="3"/>
+      <c r="S163" s="3"/>
+      <c r="T163" s="3"/>
+      <c r="U163" s="3"/>
+      <c r="V163" s="3"/>
+      <c r="W163" s="3"/>
+      <c r="X163" s="3"/>
+      <c r="Y163" s="4"/>
+    </row>
+    <row r="164" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>1</v>
+      </c>
+      <c r="B164" t="s">
+        <v>610</v>
+      </c>
+      <c r="C164" t="s">
+        <v>2</v>
+      </c>
+      <c r="D164" t="s">
+        <v>3</v>
+      </c>
+      <c r="E164" t="s">
+        <v>4</v>
+      </c>
+      <c r="F164" t="s">
+        <v>5</v>
+      </c>
+      <c r="G164" t="s">
+        <v>6</v>
+      </c>
+      <c r="H164" t="s">
+        <v>7</v>
+      </c>
+      <c r="I164" t="s">
+        <v>8</v>
+      </c>
+      <c r="J164" t="s">
+        <v>9</v>
+      </c>
+      <c r="K164" t="s">
+        <v>10</v>
+      </c>
+      <c r="L164" t="s">
+        <v>11</v>
+      </c>
+      <c r="M164" t="s">
+        <v>12</v>
+      </c>
+      <c r="N164" t="s">
+        <v>13</v>
+      </c>
+      <c r="O164" t="s">
+        <v>14</v>
+      </c>
+      <c r="P164" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q164" t="s">
+        <v>16</v>
+      </c>
+      <c r="R164" t="s">
+        <v>17</v>
+      </c>
+      <c r="S164" t="s">
+        <v>18</v>
+      </c>
+      <c r="T164" t="s">
+        <v>19</v>
+      </c>
+      <c r="U164" t="s">
+        <v>20</v>
+      </c>
+      <c r="V164" t="s">
+        <v>21</v>
+      </c>
+      <c r="W164" t="s">
+        <v>22</v>
+      </c>
+      <c r="X164" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y164" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z164" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="165" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>1</v>
+      </c>
+      <c r="B165" t="s">
+        <v>602</v>
+      </c>
+      <c r="C165">
+        <v>200</v>
+      </c>
+      <c r="D165">
+        <v>8</v>
+      </c>
+      <c r="E165" t="s">
+        <v>250</v>
+      </c>
+      <c r="F165" t="s">
+        <v>250</v>
+      </c>
+      <c r="G165">
+        <v>1</v>
+      </c>
+      <c r="H165" t="s">
+        <v>449</v>
+      </c>
+      <c r="I165">
+        <v>64</v>
+      </c>
+      <c r="J165">
+        <v>0</v>
+      </c>
+      <c r="K165">
+        <v>128</v>
+      </c>
+      <c r="L165" t="s">
+        <v>27</v>
+      </c>
+      <c r="M165" t="s">
+        <v>28</v>
+      </c>
+      <c r="N165" t="s">
+        <v>29</v>
+      </c>
+      <c r="O165" t="s">
+        <v>269</v>
+      </c>
+      <c r="P165">
+        <v>2</v>
+      </c>
+      <c r="Q165" t="s">
+        <v>31</v>
+      </c>
+      <c r="R165" t="s">
+        <v>442</v>
+      </c>
+      <c r="S165" t="s">
+        <v>606</v>
+      </c>
+      <c r="T165" t="s">
+        <v>607</v>
+      </c>
+      <c r="U165" t="s">
+        <v>608</v>
+      </c>
+      <c r="V165" t="s">
+        <v>609</v>
+      </c>
+      <c r="W165" t="s">
+        <v>37</v>
+      </c>
+      <c r="X165" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y165" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z165" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="17">
+  <tableParts count="18">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -13186,6 +13462,7 @@
     <tablePart r:id="rId16"/>
     <tablePart r:id="rId17"/>
     <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>